<commit_message>
Updating requirements change metric sheet, requirements list.
</commit_message>
<xml_diff>
--- a/documents/requirements.xlsx
+++ b/documents/requirements.xlsx
@@ -70,7 +70,7 @@
     <t>Allow filtering of devices</t>
   </si>
   <si>
-    <t>Allow filtering of devices shown on map, based on MSP, risk (highest or lowest), location, etc.</t>
+    <t>Allow filtering of devices shown on map by risk (all devices, medium-up risk, high-up risk). No filtering for mobile devices.</t>
   </si>
   <si>
     <t>No</t>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>Accept requests from Datto to add/modify/remove devices.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Internal web view - Login (Admin)</t>
+  </si>
+  <si>
+    <t>Login to web view using MSP ID &amp; password through Dattos API for Datto employees. This will login users through an admin account. No need to worry about registration.</t>
   </si>
   <si>
     <t>No</t>
@@ -230,7 +239,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -504,12 +513,22 @@
       </c>
     </row>
     <row customHeight="1" r="15" ht="12.75">
-      <c s="4" r="A15"/>
-      <c s="3" r="B15"/>
-      <c s="4" r="C15"/>
-      <c s="3" r="D15"/>
+      <c s="4" r="A15">
+        <v>14.0</v>
+      </c>
+      <c t="s" s="4" r="B15">
+        <v>45</v>
+      </c>
+      <c t="s" s="4" r="C15">
+        <v>46</v>
+      </c>
+      <c s="4" r="D15">
+        <v>0.0</v>
+      </c>
       <c s="3" r="E15"/>
-      <c s="4" r="F15"/>
+      <c t="s" s="4" r="F15">
+        <v>47</v>
+      </c>
     </row>
     <row customHeight="1" r="16" ht="12.75">
       <c s="3" r="A16"/>

</xml_diff>